<commit_message>
Add support for more Mitel devices
</commit_message>
<xml_diff>
--- a/frontend/public/device-upload-template.xlsx
+++ b/frontend/public/device-upload-template.xlsx
@@ -5,7 +5,7 @@
   <sheets>
     <sheet state="visible" name="Devices" sheetId="1" r:id="rId4"/>
     <sheet state="hidden" name="Gold Template" sheetId="2" r:id="rId5"/>
-    <sheet state="hidden" name="Device Models" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Device Models" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>Extension</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>Cisco CP-8861 Desk Phone</t>
+  </si>
+  <si>
+    <t>Mitel 6920</t>
+  </si>
+  <si>
+    <t>Mitel 6930</t>
+  </si>
+  <si>
+    <t>Mitel 6940</t>
+  </si>
+  <si>
+    <t>Mitel IP 480</t>
+  </si>
+  <si>
+    <t>Mitel IP 480g</t>
+  </si>
+  <si>
+    <t>Mitel 485g</t>
   </si>
   <si>
     <t>Mitel 6905 IP Phone</t>
@@ -232,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -245,9 +263,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -3114,7 +3135,7 @@
   </conditionalFormatting>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B658">
-      <formula1>'Device Models'!$A$1:$A$82</formula1>
+      <formula1>'Device Models'!$A$1:$A$88</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -3183,14 +3204,14 @@
     <row r="2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="7"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
+      <c r="C3" s="7"/>
       <c r="F3" s="6"/>
     </row>
     <row r="4">
@@ -5752,7 +5773,7 @@
   </conditionalFormatting>
   <dataValidations>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B658">
-      <formula1>'Device Models'!$A$1:$A$82</formula1>
+      <formula1>'Device Models'!$A$1:$A$88</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -5773,413 +5794,443 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="7" t="s">
-        <v>38</v>
+      <c r="A41" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="7" t="s">
-        <v>39</v>
+      <c r="A42" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="7" t="s">
-        <v>40</v>
+      <c r="A43" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="7" t="s">
-        <v>40</v>
+      <c r="A44" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="7" t="s">
-        <v>41</v>
+      <c r="A45" s="8" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="7" t="s">
-        <v>41</v>
+      <c r="A46" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="7" t="s">
-        <v>41</v>
+      <c r="A47" s="8" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="7" t="s">
-        <v>42</v>
+      <c r="A48" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="7" t="s">
-        <v>42</v>
+      <c r="A49" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="7" t="s">
-        <v>42</v>
+      <c r="A50" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="7" t="s">
-        <v>43</v>
+      <c r="A51" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="7" t="s">
-        <v>43</v>
+      <c r="A52" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="7" t="s">
-        <v>43</v>
+      <c r="A53" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="7" t="s">
-        <v>44</v>
+      <c r="A54" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="7" t="s">
-        <v>45</v>
+      <c r="A55" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="7" t="s">
-        <v>46</v>
+      <c r="A56" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="7" t="s">
-        <v>47</v>
+      <c r="A57" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="7" t="s">
-        <v>47</v>
+      <c r="A58" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="7" t="s">
-        <v>47</v>
+      <c r="A59" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="7" t="s">
-        <v>48</v>
+      <c r="A60" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="7" t="s">
-        <v>48</v>
+      <c r="A61" s="8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="7" t="s">
-        <v>48</v>
+      <c r="A62" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="7" t="s">
-        <v>49</v>
+      <c r="A63" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="7" t="s">
-        <v>49</v>
+      <c r="A64" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="7" t="s">
-        <v>49</v>
+      <c r="A65" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="7" t="s">
-        <v>50</v>
+      <c r="A66" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="7" t="s">
-        <v>50</v>
+      <c r="A67" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="7" t="s">
-        <v>50</v>
+      <c r="A68" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="7" t="s">
-        <v>51</v>
+      <c r="A69" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="7" t="s">
-        <v>51</v>
+      <c r="A70" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="7" t="s">
-        <v>51</v>
+      <c r="A71" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="7" t="s">
-        <v>52</v>
+      <c r="A72" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="7" t="s">
-        <v>52</v>
+      <c r="A73" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="7" t="s">
-        <v>52</v>
+      <c r="A74" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="7" t="s">
-        <v>53</v>
+      <c r="A75" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="7" t="s">
-        <v>53</v>
+      <c r="A76" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="7" t="s">
-        <v>53</v>
+      <c r="A77" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="7" t="s">
-        <v>53</v>
+      <c r="A78" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="7" t="s">
-        <v>54</v>
+      <c r="A79" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="7" t="s">
-        <v>54</v>
+      <c r="A80" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="7" t="s">
-        <v>54</v>
+      <c r="A81" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="7" t="s">
-        <v>54</v>
+      <c r="A82" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve Mitel device support
</commit_message>
<xml_diff>
--- a/frontend/public/device-upload-template.xlsx
+++ b/frontend/public/device-upload-template.xlsx
@@ -5,7 +5,7 @@
   <sheets>
     <sheet state="visible" name="Devices" sheetId="1" r:id="rId4"/>
     <sheet state="hidden" name="Gold Template" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Device Models" sheetId="3" r:id="rId6"/>
+    <sheet state="hidden" name="Device Models" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -72,7 +72,7 @@
     <t>Mitel IP 480g</t>
   </si>
   <si>
-    <t>Mitel 485g</t>
+    <t>Mitel IP 485g</t>
   </si>
   <si>
     <t>Mitel 6905 IP Phone</t>

</xml_diff>